<commit_message>
21Jun2024-aws+mysql-all button & pyspark working
</commit_message>
<xml_diff>
--- a/_raw/aws_validationcheck.xlsx
+++ b/_raw/aws_validationcheck.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://infoblox-my.sharepoint.com/personal/kkrishna_infoblox_com/Documents/hackthon-2024/Project/code-hackathon-2024/_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{726451EE-D1E4-3C48-A8A9-82A8ADD5764B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB52ADAE-FE8E-5B4E-9BDA-DA22AD05E7FC}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{726451EE-D1E4-3C48-A8A9-82A8ADD5764B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A7F0BCF-5BC2-EB40-9147-AB2F0BA4F2A0}"/>
   <bookViews>
-    <workbookView xWindow="7520" yWindow="5500" windowWidth="32520" windowHeight="17440" activeTab="2" xr2:uid="{D5DEAD4E-A5DD-6F4D-A59C-43A0FD45CE6D}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="51200" windowHeight="31520" activeTab="2" xr2:uid="{D5DEAD4E-A5DD-6F4D-A59C-43A0FD45CE6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>table_name</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>edw_test</t>
-  </si>
-  <si>
-    <t>enployee</t>
   </si>
   <si>
     <t>employee</t>
@@ -157,6 +154,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -478,9 +479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFDAE400-A446-4F41-94BD-522CD40B1D74}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView zoomScale="165" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView zoomScale="229" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -560,7 +559,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -576,17 +575,17 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.6640625" customWidth="1"/>
+    <col min="3" max="3" width="55.83203125" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.5" customWidth="1"/>
+    <col min="6" max="6" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -614,7 +613,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>11</v>

</xml_diff>